<commit_message>
Part 4 Scaffold complete
</commit_message>
<xml_diff>
--- a/timesheet_DanielWilson_s266070.xlsx
+++ b/timesheet_DanielWilson_s266070.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\GitHub\S220PRT585_s266070\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADB5A4C-D9FC-415A-AF35-D12D64FE6A28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40F856D-3E44-49F5-AF1E-60AD0EEAB3EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{471AB8EC-D1D5-41D0-B4E5-27338561C4E5}"/>
+    <workbookView xWindow="660" yWindow="450" windowWidth="21600" windowHeight="11385" xr2:uid="{471AB8EC-D1D5-41D0-B4E5-27338561C4E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Week 1</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>Started the MVC Tutorial</t>
+  </si>
+  <si>
+    <t>Teeam meeting we complained about the tutorials being poorly written and we discussed what problems we had encountered</t>
+  </si>
+  <si>
+    <t>Continued the MVC Tutorial</t>
+  </si>
+  <si>
+    <t>Continued working on MVC Tutorial</t>
   </si>
 </sst>
 </file>
@@ -672,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB8FECF-62AE-4913-A869-EE2F5B95DB99}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,9 +769,15 @@
       <c r="E2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>

</xml_diff>

<commit_message>
Part 8 Pre SQL modification
</commit_message>
<xml_diff>
--- a/timesheet_DanielWilson_s266070.xlsx
+++ b/timesheet_DanielWilson_s266070.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\GitHub\S220PRT585_s266070\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drac1\Documents\GitHub\S220PRT585_s266070\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696542AF-0ED9-4031-A0C4-C283508634CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137CE1A5-45A3-48B9-BC37-5B5C5488728C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="450" windowWidth="21600" windowHeight="11385" xr2:uid="{471AB8EC-D1D5-41D0-B4E5-27338561C4E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{471AB8EC-D1D5-41D0-B4E5-27338561C4E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Week 1</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Got github up to scratch, relearnt how to use excel, got timesheet formatted, and installed visual studio.</t>
   </si>
   <si>
-    <t>Continued the MVC Tutorial</t>
-  </si>
-  <si>
     <t>Continued working on MVC Tutorial. Part 4 was plauged by Capitalisation problems.</t>
   </si>
   <si>
@@ -162,6 +159,12 @@
   </si>
   <si>
     <t>Continued the MVC Tutorial.</t>
+  </si>
+  <si>
+    <t>Continued working on MVC tutorial.</t>
+  </si>
+  <si>
+    <t>Team meeting to try and resolve andy's error and finish the Tutorial.</t>
   </si>
 </sst>
 </file>
@@ -690,16 +693,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB8FECF-62AE-4913-A869-EE2F5B95DB99}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="21" width="30.7109375" customWidth="1"/>
+    <col min="2" max="21" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="8" t="s">
         <v>13</v>
@@ -762,7 +765,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -773,30 +776,33 @@
         <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="L2" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -805,7 +811,7 @@
       <c r="T2" s="2"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -830,7 +836,7 @@
       <c r="T3" s="2"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -855,7 +861,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -880,7 +886,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -905,7 +911,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="3"/>
     </row>
-    <row r="7" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -930,7 +936,7 @@
       <c r="T7" s="2"/>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -955,7 +961,7 @@
       <c r="T8" s="2"/>
       <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -980,7 +986,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="3"/>
     </row>
-    <row r="10" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1005,7 +1011,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="3"/>
     </row>
-    <row r="11" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -1030,7 +1036,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="3"/>
     </row>
-    <row r="12" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -1055,7 +1061,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -1080,7 +1086,7 @@
       <c r="T13" s="2"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -1105,7 +1111,7 @@
       <c r="T14" s="4"/>
       <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Part 10 Complete & timesheet updated
</commit_message>
<xml_diff>
--- a/timesheet_DanielWilson_s266070.xlsx
+++ b/timesheet_DanielWilson_s266070.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drac1\Documents\GitHub\S220PRT585_s266070\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137CE1A5-45A3-48B9-BC37-5B5C5488728C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0395BF-F28A-447A-9F86-830288D70BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{471AB8EC-D1D5-41D0-B4E5-27338561C4E5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Week 1</t>
   </si>
@@ -158,13 +158,16 @@
     <t>Started the MVC Tutorial.</t>
   </si>
   <si>
-    <t>Continued the MVC Tutorial.</t>
-  </si>
-  <si>
-    <t>Continued working on MVC tutorial.</t>
-  </si>
-  <si>
     <t>Team meeting to try and resolve andy's error and finish the Tutorial.</t>
+  </si>
+  <si>
+    <t>Finished MVC tutorial.</t>
+  </si>
+  <si>
+    <t>Continued the MVC Tutorial. Moved tutorial from group repository to personal one.</t>
+  </si>
+  <si>
+    <t>Team meeting continued. Helped and with SQL issues.</t>
   </si>
 </sst>
 </file>
@@ -694,7 +697,7 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,7 +785,7 @@
         <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>37</v>
@@ -800,9 +803,11 @@
         <v>42</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>

</xml_diff>

<commit_message>
Movie manager project craeted
</commit_message>
<xml_diff>
--- a/timesheet_DanielWilson_s266070.xlsx
+++ b/timesheet_DanielWilson_s266070.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drac1\Documents\GitHub\S220PRT585_s266070\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\GitHub\S220PRT585_s266070\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7B582D-F180-413C-B154-F3EAFEFAAC11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3949CA4B-A217-41E8-9936-2141A469F441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{471AB8EC-D1D5-41D0-B4E5-27338561C4E5}"/>
+    <workbookView xWindow="660" yWindow="450" windowWidth="21600" windowHeight="11385" xr2:uid="{471AB8EC-D1D5-41D0-B4E5-27338561C4E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Week 1</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>In person team meeting to try and resolve andy's error and finish the Tutorial.</t>
+  </si>
+  <si>
+    <t>Figuring out the connection string and conferming it works. Had problems with week 1 tutorial work caused by moving work from PC to laptop and back again.</t>
+  </si>
+  <si>
+    <t>Team meeting talked about problems with database migrations not working.</t>
+  </si>
+  <si>
+    <t>Researched Tag Helpers</t>
   </si>
 </sst>
 </file>
@@ -364,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -396,6 +405,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,16 +725,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB8FECF-62AE-4913-A869-EE2F5B95DB99}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="21" width="30.6640625" customWidth="1"/>
+    <col min="2" max="21" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="8" t="s">
         <v>13</v>
@@ -785,7 +797,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -836,13 +848,19 @@
       <c r="T2" s="2"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -861,7 +879,7 @@
       <c r="T3" s="2"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -886,7 +904,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -911,7 +929,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -936,7 +954,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="3"/>
     </row>
-    <row r="7" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -961,7 +979,7 @@
       <c r="T7" s="2"/>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -986,7 +1004,7 @@
       <c r="T8" s="2"/>
       <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1011,7 +1029,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="3"/>
     </row>
-    <row r="10" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1036,7 +1054,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="3"/>
     </row>
-    <row r="11" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -1061,7 +1079,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="3"/>
     </row>
-    <row r="12" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -1086,7 +1104,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -1111,7 +1129,7 @@
       <c r="T13" s="2"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -1136,7 +1154,7 @@
       <c r="T14" s="4"/>
       <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Everything except catagory dropdown finished
</commit_message>
<xml_diff>
--- a/timesheet_DanielWilson_s266070.xlsx
+++ b/timesheet_DanielWilson_s266070.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\GitHub\S220PRT585_s266070\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4FFCEA-8C11-4E73-A244-C963A3DC1650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD04F48D-863D-48B7-A067-665001E7B048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="450" windowWidth="21600" windowHeight="11385" xr2:uid="{471AB8EC-D1D5-41D0-B4E5-27338561C4E5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Week 1</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Team meeting</t>
+  </si>
+  <si>
+    <t>Team meeting continuted. Guzzi has problems with his enum.</t>
   </si>
 </sst>
 </file>
@@ -731,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB8FECF-62AE-4913-A869-EE2F5B95DB99}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,11 +879,15 @@
       <c r="G3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>

</xml_diff>